<commit_message>
Subiendo imgages y cambios
</commit_message>
<xml_diff>
--- a/dist/smg-front/assets/bd/carrouselData.xlsx
+++ b/dist/smg-front/assets/bd/carrouselData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\Proyectos-Recap\plantillas\plantilla2\smgFront\src\assets\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346744BB-5C2C-4EBF-A248-FB42628535CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936CE170-334B-4100-BE53-37032F3D88CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{A005A446-4FBB-42A9-BE7A-84389F7F20C8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>nombre</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>red</t>
+  </si>
+  <si>
+    <t>SMG</t>
+  </si>
+  <si>
+    <t>Hola somos talalalsaldafasfalsf</t>
+  </si>
+  <si>
+    <t>asfsagfasdgadsgasdgadsgasdgadg</t>
+  </si>
+  <si>
+    <t>agadsgadgagadgadgasfrwqfSCs</t>
   </si>
 </sst>
 </file>
@@ -469,7 +481,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,11 +514,15 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
@@ -516,11 +532,15 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
@@ -530,11 +550,15 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>

</xml_diff>